<commit_message>
Atualizando informações do projeto
Atualizando informações do projeto
</commit_message>
<xml_diff>
--- a/Requisitos/Template_Projeto_SISMAT.xlsx
+++ b/Requisitos/Template_Projeto_SISMAT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>CAMPO</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>&lt;aluno 4&gt;</t>
+  </si>
+  <si>
+    <t>SISMAT-SISTEMA DE MATRICULA</t>
   </si>
 </sst>
 </file>
@@ -645,6 +648,18 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -685,18 +700,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1660,7 +1663,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1680,17 +1683,19 @@
       <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="62" t="s">
+      <c r="B1" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="54" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="56" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="1"/>
@@ -1907,13 +1912,13 @@
       <c r="A2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="68"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="70"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2125,16 +2130,16 @@
       <c r="HI2" s="1"/>
     </row>
     <row r="3" spans="1:217" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="54"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="70"/>
+      <c r="H3" s="56"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -2346,14 +2351,14 @@
       <c r="HI3" s="1"/>
     </row>
     <row r="4" spans="1:217" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="61"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="69"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="55"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="71"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>

</xml_diff>